<commit_message>
rebild bot with tlebot lib., rebild xlsx-parser and sites parser
</commit_message>
<xml_diff>
--- a/urls/urls.xlsx
+++ b/urls/urls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -34,24 +34,55 @@
     <t xml:space="preserve">instr_urls</t>
   </si>
   <si>
-    <t xml:space="preserve">Какле-то название</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-bosch-zelenyi/akkumulatornyj-surupovert-bosch-psr-1440li-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-powermaxx-bs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-331-dwye</t>
+    <t xml:space="preserve">price_strbt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price_instr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000019707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая "GWS 22-230 JH" (Bosch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://stroybatinfo.ru/catalog/113/5864/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-230-jh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000018378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая "GWS 22-230 H" (Bosch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://stroybatinfo.ru/catalog/113/5863/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-230h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000021170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая "GWS 22-180 H" (Bosch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://stroybatinfo.ru/catalog/113/5861/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-180-h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -125,13 +156,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -151,19 +190,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -175,39 +215,63 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-bosch-zelenyi/akkumulatornyj-surupovert-bosch-psr-1440li-2"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-powermaxx-bs"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-331-dwye"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://stroybatinfo.ru/catalog/113/5864/"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-230-jh"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://stroybatinfo.ru/catalog/113/5863/"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-230h"/>
+    <hyperlink ref="C4" r:id="rId5" display="https://stroybatinfo.ru/catalog/113/5861/"/>
+    <hyperlink ref="D4" r:id="rId6" display="https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/shlifmashina-uglovaya-bosch-gws-22-180-h"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add new urls to check
</commit_message>
<xml_diff>
--- a/urls/urls.xlsx
+++ b/urls/urls.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="1021">
   <si>
     <t>id</t>
   </si>
@@ -1372,6 +1372,1716 @@
   </si>
   <si>
     <t>https://stroybatinfo.ru/catalog/82/379494/</t>
+  </si>
+  <si>
+    <t>21037</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 5030" (Makita)</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/slifmasina-uglovaa-makita-ga-5030-x3</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/5973/</t>
+  </si>
+  <si>
+    <t>33945</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 4530" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/130820/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-4530</t>
+  </si>
+  <si>
+    <t>14440</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9565 НZ" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/97938/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-9565-nz</t>
+  </si>
+  <si>
+    <t>89493</t>
+  </si>
+  <si>
+    <t>Ш/м угловая "9558 HPG" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/115640/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/slifmasina-uglovaa-makita-9558hpg</t>
+  </si>
+  <si>
+    <t>89673</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9558 HNK6" (Makita) 840 Вт., 125 мм., 10000 об/мин., 1,6 кг. пластиковый кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/115710/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-9558-nnk</t>
+  </si>
+  <si>
+    <t>33037</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9558 HNK" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/100821/</t>
+  </si>
+  <si>
+    <t>13887</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9557 HN01" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/5970/</t>
+  </si>
+  <si>
+    <t>1559</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9069" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/5967/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-9069</t>
+  </si>
+  <si>
+    <t>52987</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "9069 F" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/260598/</t>
+  </si>
+  <si>
+    <t>74425</t>
+  </si>
+  <si>
+    <t>Шлифмашина прямая "GD 0800C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/112/4613354/</t>
+  </si>
+  <si>
+    <t>73091</t>
+  </si>
+  <si>
+    <t>Шлифмашина полировальная "SA 5040 C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/111/5800238/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-5040c</t>
+  </si>
+  <si>
+    <t>1574</t>
+  </si>
+  <si>
+    <t>Шлифмашина ленточная "9911" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/110/5966/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-lentochnye/tm-makita/shlifmashina-lentochnaya-makita-9911</t>
+  </si>
+  <si>
+    <t>2041</t>
+  </si>
+  <si>
+    <t>Шлифмашина ленточная "9910" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/110/5965/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-lentochnye/tm-makita/shlifmashina-lentochnaya-makita-9910</t>
+  </si>
+  <si>
+    <t>22159</t>
+  </si>
+  <si>
+    <t>Шлифмашина вибрационная "ВО 3711" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/107/5962/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ploskoshlifovalnye/tm-makita/shlifmashina-ploskoshlifovalnaya-makita-bo-3711</t>
+  </si>
+  <si>
+    <t>24175</t>
+  </si>
+  <si>
+    <t>Шлифмашина вибрационная "ВО 3710" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/107/5961/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ploskoshlifovalnye/tm-makita/shlifmashina-ploskoshlifovalnaya-makita-bo-3710</t>
+  </si>
+  <si>
+    <t>40245</t>
+  </si>
+  <si>
+    <t>Фрезер "RT 0700CX2" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/242277/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/frezery/tm-makita/frezer-kromocnyj-makita-rt0700cx2</t>
+  </si>
+  <si>
+    <t>80559</t>
+  </si>
+  <si>
+    <t>Фрезер "RT 0700C" (Makita) 710 Вт, 10000-30000 об/мин., цанга 6-8 мм., 1,8 кг, коробка, прямая направляющая.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/98867/</t>
+  </si>
+  <si>
+    <t>44570</t>
+  </si>
+  <si>
+    <t>Фрезер "RP 2301 FCX" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/249476/</t>
+  </si>
+  <si>
+    <t>37443</t>
+  </si>
+  <si>
+    <t>Фрезер "RP 2300 FC" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/240851/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/frezery/tm-makita/frezer-makita-rp-2300-fc</t>
+  </si>
+  <si>
+    <t>79727</t>
+  </si>
+  <si>
+    <t>Фрезер "RP 1801 F" (Makita) 1650 Вт, 22000 об/мин., ход 0-70 мм., цанга 12 мм., 6 кг, плавный пуск</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/97181/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/frezery/tm-makita/frezer-makita-rp-1801-f</t>
+  </si>
+  <si>
+    <t>1131</t>
+  </si>
+  <si>
+    <t>Фрезер "RP 1110 C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/5959/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/frezery/tm-makita/frezer-makita-rp-1110-c</t>
+  </si>
+  <si>
+    <t>72932</t>
+  </si>
+  <si>
+    <t>Фрезер "RP 0900" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/3303463/</t>
+  </si>
+  <si>
+    <t>46078</t>
+  </si>
+  <si>
+    <t>Фрезер "3612С" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/251425/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/frezery/tm-makita/frezer-makita-3612-s</t>
+  </si>
+  <si>
+    <t>51569</t>
+  </si>
+  <si>
+    <t>Устройство воздуходувное "UB1103" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/234/257202/</t>
+  </si>
+  <si>
+    <t>65725</t>
+  </si>
+  <si>
+    <t>Труборез "LW1400" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/96/383715/</t>
+  </si>
+  <si>
+    <t>83175</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. ударный "DTD 154 Z" (Makita) 18В, без аккумулятора и зар. устройства, 0-1100\2100\3600 об\м, 175 Нм, шестигранник 1/4", 1,5 кг, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/106140/</t>
+  </si>
+  <si>
+    <t>83173</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. ударный "DTD 154 RFE" (Makita) 18В, 2х3АчLi-ion, 0-1100\2100\3600 об\м, 175 Нм, шестигранник 1/4", 1,5 кг, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/106139/</t>
+  </si>
+  <si>
+    <t>32197</t>
+  </si>
+  <si>
+    <t>Шуруповерт сетевой "TD0101F" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/116/97351/</t>
+  </si>
+  <si>
+    <t>57570</t>
+  </si>
+  <si>
+    <t>Шуруповерт сетевой "TD0101" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/116/263801/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-setevye/tm-makita/udarnyi-shurupovert-makita-td-0101</t>
+  </si>
+  <si>
+    <t>81136</t>
+  </si>
+  <si>
+    <t>Шуруповерт сетевой ударный "TD0100" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/116/100125/</t>
+  </si>
+  <si>
+    <t>89494</t>
+  </si>
+  <si>
+    <t>Шуруповерт сетевой "DF0300" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/116/115641/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-setevye/tm-makita/surupovert-makita-df0300</t>
+  </si>
+  <si>
+    <t>72674</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DF 457 DWLE" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/2983550/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-457-dwle</t>
+  </si>
+  <si>
+    <t>67923</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DF 457 DWE" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/386651/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-457-dwe</t>
+  </si>
+  <si>
+    <t>67920</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DF 347 DWE" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/386649/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-347-dwe</t>
+  </si>
+  <si>
+    <t>90344</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DF 333 DWYE" (Makita) 12 В, Li-Ion, 0-450/1700 об/мин, 14-30 Hm, БЗП 10 мм, 2 акк Li-Ion 1,5 ah, 1,1 кг, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/116059/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulatornyj-surupovert-makita-df-333-dwye</t>
+  </si>
+  <si>
+    <t>62806</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DF 331 DWYE" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/380839/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-df-331-dwye</t>
+  </si>
+  <si>
+    <t>63822</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DDF 481 RTE" (Makita) 18 В, Li-Ion, 2 аккум. 5 Ач, б/щеточный двигатель, 0-550/2100 об/мин, 60-115 Hm, БЗП 13 мм, 2.6 кг, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/380219/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-ddf-481-rte</t>
+  </si>
+  <si>
+    <t>63820</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DDF 480 RME" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/380218/</t>
+  </si>
+  <si>
+    <t>73224</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DDF 453 RFE" (Makita) 18 В, Li-Ion, 0-400/0-1300 об/мин, 27-42 Hm, БЗП 13 мм, 2 акк, 3.0 ah, кейс, 1,8 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/95933/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-makita/akkumulyatornyi-shurupovert-makita-ddf-453-rfe</t>
+  </si>
+  <si>
+    <t>69962</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "DDF 451 RFE" (Makita) 18В,2х3АчLi-ion,БЗП-13мм,0-300\0-600\0-1700об\м,80\40Нм,2.1кг,чем,подсв,совмест с 4АчLi-ion</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/98475/</t>
+  </si>
+  <si>
+    <t>37610</t>
+  </si>
+  <si>
+    <t>Шлифмашина эксцентриковая "ВО 5031" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/114/240854/</t>
+  </si>
+  <si>
+    <t>27791</t>
+  </si>
+  <si>
+    <t>Шлифмашина эксцентриковая "ВО 5030" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/114/35525/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ekstsentrikovye/tm-makita/shlifmashina-ekstsentrikovaya-makita-bo-5030</t>
+  </si>
+  <si>
+    <t>31612</t>
+  </si>
+  <si>
+    <t>Шлифмашина щеточная "9741" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/110/132105/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-shchetochnye/tm-makita/shlifmashina-shchetochnaya-makita-9741</t>
+  </si>
+  <si>
+    <t>80505</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая аккум. "DGA504RF" (Makita) 18В, аккумулятор 1х3Ач Li-ion, 125 мм.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1045/98868/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye-akkumulyatornye/tm-makita/akkumulatornaa-uglovaa-slifmasina-makita-dga-504-rf</t>
+  </si>
+  <si>
+    <t>32364</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 9050 " (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/98230/</t>
+  </si>
+  <si>
+    <t>5502</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 9020 " (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/7965/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-9020</t>
+  </si>
+  <si>
+    <t>5256</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 9020 SF" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/87229/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-9020-sf</t>
+  </si>
+  <si>
+    <t>35452</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 7050" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/132104/</t>
+  </si>
+  <si>
+    <t>29497</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 6021 С" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/87396/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-6021-s</t>
+  </si>
+  <si>
+    <t>90225</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 5040R" (Makita) 1100 Вт, 125 мм, 11000 об/м, муфта SJSII,anti-restart, плавный пуск 2.5 кг, коробка.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/115945/</t>
+  </si>
+  <si>
+    <t>64821</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 5034" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/380835/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-makita/shlifmashina-uglovaya-makita-ga-5034</t>
+  </si>
+  <si>
+    <t>34790</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GA 5030К" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/130821/</t>
+  </si>
+  <si>
+    <t>63877</t>
+  </si>
+  <si>
+    <t>Перфоратор "HR 4003 C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/92/380201/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-max/tm-makita/perforator-sds-max-makita-hr-4003-s</t>
+  </si>
+  <si>
+    <t>11014</t>
+  </si>
+  <si>
+    <t>Перфоратор "HR 2470" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5934/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-makita/perforator-sds-makita-hr-2470</t>
+  </si>
+  <si>
+    <t>11015</t>
+  </si>
+  <si>
+    <t>Перфоратор "HR 2470 FT" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5933/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-makita/perforator-sds-makita-hr-2470-ft</t>
+  </si>
+  <si>
+    <t>32222</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "HМ 1203 С" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/97679/</t>
+  </si>
+  <si>
+    <t>73023</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "HМ 1101 С" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/3303456/</t>
+  </si>
+  <si>
+    <t>29293</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "HМ 0870 С" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/88123/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/molotki-otboinye/tm-makita/molotok-otboinyi-makita-hm-0870-c</t>
+  </si>
+  <si>
+    <t>32304</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная "JR 3060 T" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/99/98214/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/sabelnye-pily-setevye/tm-makita/elektropila-sabelnaa-makita-jr-3060-t</t>
+  </si>
+  <si>
+    <t>73090</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная "JR 3050 T" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/99/3303455/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/sabelnye-pily-setevye/tm-makita/elektropila-sabelnaa-makita-jr-3050-t</t>
+  </si>
+  <si>
+    <t>41545</t>
+  </si>
+  <si>
+    <t>Ножницы листовые "JS 1602" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/90/244746/</t>
+  </si>
+  <si>
+    <t>12187</t>
+  </si>
+  <si>
+    <t>Лобзик "4350 FCT" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/18667/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4350-fct</t>
+  </si>
+  <si>
+    <t>33944</t>
+  </si>
+  <si>
+    <t>Лобзик "4350 CT" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/130818/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4350-ct</t>
+  </si>
+  <si>
+    <t>10842</t>
+  </si>
+  <si>
+    <t>Лобзик "4329" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/5925/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4329-kh1</t>
+  </si>
+  <si>
+    <t>32274</t>
+  </si>
+  <si>
+    <t>Лобзик "4329 K" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/98211/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4329-kx1</t>
+  </si>
+  <si>
+    <t>10841</t>
+  </si>
+  <si>
+    <t>Лобзик "4327" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/5924/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4327</t>
+  </si>
+  <si>
+    <t>12908</t>
+  </si>
+  <si>
+    <t>Лобзик "4326" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/18666/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-makita/lobzik-makita-4326</t>
+  </si>
+  <si>
+    <t>1595</t>
+  </si>
+  <si>
+    <t>Дрель ударная "HP 2050" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/18665/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-makita/drel-udarnaya-makita-nr-2050</t>
+  </si>
+  <si>
+    <t>22550</t>
+  </si>
+  <si>
+    <t>Дрель ударная "HP 1640 " (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/5919/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-makita/drel-udarnaya-makita-hp-1640</t>
+  </si>
+  <si>
+    <t>26651</t>
+  </si>
+  <si>
+    <t>Дрель "DP 4010 " (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/35695/</t>
+  </si>
+  <si>
+    <t>10736</t>
+  </si>
+  <si>
+    <t>Дрель "6413" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/89453/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-makita/drel-makita-6413</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>Дрель "6408" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/5915/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-makita/drel-makita-6408</t>
+  </si>
+  <si>
+    <t>87928</t>
+  </si>
+  <si>
+    <t>Гайковерт акк."DTW 285 RFJX" (Makita) BL-мотор (бесщеточный), 18 В, 2х3 Ач Li-Ion, 0-1800/2600/3500 уд/мин, 280 Нм, хвостовик 1/2", 1,7 кг, подсветка, набор головок, кейс MakPac.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/115095/</t>
+  </si>
+  <si>
+    <t>69478</t>
+  </si>
+  <si>
+    <t>Гайковерт акк."DTW 1001 RTJ" (Makita) 18 В, бесщеточный двигатель, 2х5 Ач Li-Ion, 0-900/1000/1800 об/мин, 0-1800/2000/2200 уд/мин, 1050 Нм, наружный квадрат 3/4", 3,4 кг, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/95931/</t>
+  </si>
+  <si>
+    <t>11071</t>
+  </si>
+  <si>
+    <t>Гайковерт ударный "TW1000" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/36947/</t>
+  </si>
+  <si>
+    <t>2043</t>
+  </si>
+  <si>
+    <t>Гайковерт ударный "TW0350" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/86536/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/gaikoverty/gaikoverty-setevye/tm-makita/gaikovert-udarnyi-makita-tw0350</t>
+  </si>
+  <si>
+    <t>13174</t>
+  </si>
+  <si>
+    <t>Гайковерт ударный "TW0200" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/87778/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/gaikoverty/gaikoverty-setevye/tm-makita/gaikovert-udarnyi-makita-tw0200</t>
+  </si>
+  <si>
+    <t>32368</t>
+  </si>
+  <si>
+    <t>Рубанок "KP0810C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/255591/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-setevye/tm-makita/rubanok-makita-kp-0810-c</t>
+  </si>
+  <si>
+    <t>53818</t>
+  </si>
+  <si>
+    <t>Пылесос универсальный "VC 2512L" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/151/260151/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/kliningovaya-tekhnika/pylesosy/tm-makita/pylesos-makita-vc-2512l</t>
+  </si>
+  <si>
+    <t>2034</t>
+  </si>
+  <si>
+    <t>Труборез "2414 NB" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/96/5956/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/mashiny-otreznye-po-metallu/tm-makita/otreznaya-pila-po-metallu-makita-2414-nb</t>
+  </si>
+  <si>
+    <t>4025</t>
+  </si>
+  <si>
+    <t>Гайковерт ударный "6906" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/35694/</t>
+  </si>
+  <si>
+    <t>42017</t>
+  </si>
+  <si>
+    <t>Рубанок "KP0810" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/255590/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-setevye/tm-makita/rubanok-makita-kp-0810</t>
+  </si>
+  <si>
+    <t>41546</t>
+  </si>
+  <si>
+    <t>Рубанок "KP 0800" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/255589/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-setevye/tm-makita/rubanok-makita-kp-0800</t>
+  </si>
+  <si>
+    <t>2824</t>
+  </si>
+  <si>
+    <t>Рубанок "1911 B" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/255588/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-setevye/tm-makita/rubanok-makita-1911-v</t>
+  </si>
+  <si>
+    <t>2033</t>
+  </si>
+  <si>
+    <t>Станок рейсмусный "2012 NB" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/185/60860/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/stanki-reismusovye-i-strogalnye/tm-makita/stanok-derevoobrabatyvayushchii-reismusovyi-makita-2012-nb</t>
+  </si>
+  <si>
+    <t>54013</t>
+  </si>
+  <si>
+    <t>Пылесос универсальный "VC 3011L" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/151/260333/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/kliningovaya-tekhnika/pylesosy/tm-makita/pylesos-makita-vc-3011l</t>
+  </si>
+  <si>
+    <t>51720</t>
+  </si>
+  <si>
+    <t>Пистолет горячего воздуха "HG 651 C" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/258661/</t>
+  </si>
+  <si>
+    <t>35453</t>
+  </si>
+  <si>
+    <t>Пистолет горячего воздуха "HG 551 VK" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/132103/</t>
+  </si>
+  <si>
+    <t>21020</t>
+  </si>
+  <si>
+    <t>Пистолет горячего воздуха "HG 5012К" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/5949/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/feny-stroitelnye-i-payalnye-pistolety/feny-stroitelnye/tm-makita/pistolet-goryachego-vozdukha-makita-hg-551-vk</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/feny-stroitelnye-i-payalnye-pistolety/feny-stroitelnye/tm-makita/pistolet-goryachego-vozdukha-makita-hg-5012-k</t>
+  </si>
+  <si>
+    <t>27939</t>
+  </si>
+  <si>
+    <t>Пистолет горячего воздуха "HG 5012" (Makitа)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/95840/</t>
+  </si>
+  <si>
+    <t>64860</t>
+  </si>
+  <si>
+    <t>Пила цепная "UC 4041 A" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/98/380834/</t>
+  </si>
+  <si>
+    <t>63168</t>
+  </si>
+  <si>
+    <t>Пила цепная "UC 3541 A" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/98/379500/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/vse-dlya-sada/pily-tsepnye/tsepnye-elektropily/tm-makita/elektropila-tsepnaya-makita-uc-3541-a</t>
+  </si>
+  <si>
+    <t>57571</t>
+  </si>
+  <si>
+    <t>Пила цепная "UC 3041 A" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/98/263797/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/vse-dlya-sada/pily-tsepnye/tsepnye-elektropily/tm-makita/elektropila-tsepnaya-makita-uc-3041-a</t>
+  </si>
+  <si>
+    <t>2122</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "LS 1040" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/5941/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-makita/pila-tortsovochnaya-makita-ls-1040</t>
+  </si>
+  <si>
+    <t>40424</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "LS 1018L" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/247228/</t>
+  </si>
+  <si>
+    <t>35458</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "LH 1040" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/132102/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-makita/pila-tortsovochnaya-kombinirovannaya-makita-ln-1040</t>
+  </si>
+  <si>
+    <t>63155</t>
+  </si>
+  <si>
+    <t>Пила погружная "SP6000" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/379499/</t>
+  </si>
+  <si>
+    <t>73086</t>
+  </si>
+  <si>
+    <t>Пила дисковая по алюминию"CA 5000 XJ" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/3303460/</t>
+  </si>
+  <si>
+    <t>60669</t>
+  </si>
+  <si>
+    <t>Пила дисковая "HS7601" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/326467/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-makita/pila-diskovaya-makita-hs7601</t>
+  </si>
+  <si>
+    <t>70537</t>
+  </si>
+  <si>
+    <t>Пила дисковая "HS6601" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/822828/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-makita/pila-diskovaa-makita-hs6601</t>
+  </si>
+  <si>
+    <t>37655</t>
+  </si>
+  <si>
+    <t>Пила дисковая "5477 NB" (Makita)</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-makita/pila-diskovaya-makita-5477-nb</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/229230/</t>
+  </si>
+  <si>
+    <t>21849</t>
+  </si>
+  <si>
+    <t>Пила дисковая "5008 MG" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/7964/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-makita/pila-diskovaya-makita-5008-mg</t>
+  </si>
+  <si>
+    <t>80431</t>
+  </si>
+  <si>
+    <t>Перфоратор аккумуляторный "DHR 202RF" (Makita)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1056/98474/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-akkumulyatornye/tm-makita/perforator-akkumulatornyj-makita-dhr-202-rf</t>
+  </si>
+  <si>
+    <t>66332</t>
+  </si>
+  <si>
+    <t>Перфоратор "HR 4013 C" (Makita) 1100 Вт.,SDS max, 9,5 Дж,235-480 об/мин, 6,3кг, чем.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/92/95932/</t>
+  </si>
+  <si>
+    <t>75080</t>
+  </si>
+  <si>
+    <t>Пистолет гор.воздуха "H 16-500" (Metabo) 1600Вт, расход воздуха 240/450 л/мин, 300/500 гр., , 0,6 кг, длина кабеля 2,2 м, коробка.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/6111646/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/feny-stroitelnye-i-payalnye-pistolety/feny-stroitelnye/tm-metabo/pistolet-goryachego-vozdukha-metabo-h-16-500</t>
+  </si>
+  <si>
+    <t>86132</t>
+  </si>
+  <si>
+    <t>Пистолет клеевой "KE 3000" (Metabo) стержни 11 мм, 0,25 кг, длина кабеля 1.9 м, коробка.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/100/112021/</t>
+  </si>
+  <si>
+    <t>59809</t>
+  </si>
+  <si>
+    <t>Пылесос универсальный "ASA 25 L PC" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/151/320282/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/kliningovaya-tekhnika/pylesosy/tm-metabo/pylesos-metabo-asa-25lpc</t>
+  </si>
+  <si>
+    <t>46291</t>
+  </si>
+  <si>
+    <t>Рейсмус "DH 330" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/185/343841/</t>
+  </si>
+  <si>
+    <t>74992</t>
+  </si>
+  <si>
+    <t>Рубанок "HO 26-82" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/5264666/</t>
+  </si>
+  <si>
+    <t>78328</t>
+  </si>
+  <si>
+    <t>Рубанок аккумуляторный "HO 18 LTX 20-82" (Metabo) 18В, ширина строгания 82 мм, глубина строгания до 2 мм, 16000 об/мин, без АКК и ЗУ,картон</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/83/91844/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-akkumulyatornye/tm-metabo/akkumulatornyj-rubanok-metabo-ho-18-ltx-20-82</t>
+  </si>
+  <si>
+    <t>44093</t>
+  </si>
+  <si>
+    <t>Труборез "CS 23-355" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/96/248918/</t>
+  </si>
+  <si>
+    <t>85468</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 1100-125" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/111071/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-w-1100-125</t>
+  </si>
+  <si>
+    <t>61940</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/403595/</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 12-125 Quick" (Metabo)</t>
+  </si>
+  <si>
+    <t>61941</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 2400-230" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/91846/</t>
+  </si>
+  <si>
+    <t>59781</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 750-125" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/320283/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-w-750-125</t>
+  </si>
+  <si>
+    <t>85464</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 850-125" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/111067/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-850-125</t>
+  </si>
+  <si>
+    <t>72884</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "W 9-125" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/3206813/</t>
+  </si>
+  <si>
+    <t>86720</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "WE 2200-230" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/112678/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-2200-230-2</t>
+  </si>
+  <si>
+    <t>85458</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "PowerMaxx BS 12" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/111066/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-12</t>
+  </si>
+  <si>
+    <t>85466</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "PowerMaxx BS 12 BL" (Metabo) 12 В, бесщеточная дрель, 0-500/0-1650 об/мин, 18-48Hm, БЗП 10мм, 2 акк, 2.0 Ah, кейс, 1 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/111069/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-12-bl</t>
+  </si>
+  <si>
+    <t>90069</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "BS 10,8 Li" (Metabo) 10.8 В, 0-350/0-1300 об/мин, 17-34Hm, БЗП 10 мм, 2 акк, 2.0 Ah, кейс, 0.8 кг, в комплекте набор бит и фонарь.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/115833/</t>
+  </si>
+  <si>
+    <t>72887</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "BS 18 LTX Impuls" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/3206816/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-bs18-ltx-imp</t>
+  </si>
+  <si>
+    <t>74712</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "BS 18 L" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/4798938/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-18-l</t>
+  </si>
+  <si>
+    <t>89468</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "BS 18 L BL" (Metabo) 18 В, бесщеточная дрель, 2 Li-Ion аккум. 4,0 Ач, 0-550/0-1850 об/мин, 25-60 Нм, БЗП 13 мм, кейс, 1,2 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/115628/</t>
+  </si>
+  <si>
+    <t>78329</t>
+  </si>
+  <si>
+    <t>Ш/м эксцентриковая "SXE 3125" (Metabo) 310Вт, подошва 125мм, калебательный контур 3мм, 4000-12000 об/мин, 1,5 кг, картон.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/114/91847/</t>
+  </si>
+  <si>
+    <t>72883</t>
+  </si>
+  <si>
+    <t>Шлифмашина эксцентриковая "FSX 200 Intec" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/114/3206814/</t>
+  </si>
+  <si>
+    <t>46287</t>
+  </si>
+  <si>
+    <t>Ш/м угловая "WEV 15-125 Quick" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/251757/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-wev-15-125-quick</t>
+  </si>
+  <si>
+    <t>70102</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "WEV 10-125 Quick" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/403597/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-wev-10-125-quick</t>
+  </si>
+  <si>
+    <t>73827</t>
+  </si>
+  <si>
+    <t>Гайковерт "SSW 650" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/3990313/</t>
+  </si>
+  <si>
+    <t>85467</t>
+  </si>
+  <si>
+    <t>Гайковерт аккумуляторный "PowerMaxx SSD 12 BL" (Metabo) 12 В, 2 акк * 2Ач, 0 - 2500 об/мин, 4000 уд/мин, 140 Нм, внутренний шестигранник 1/4" (6,35 мм), вес 1 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/111070/</t>
+  </si>
+  <si>
+    <t>78330</t>
+  </si>
+  <si>
+    <t>Дрель миксер "RWE 1020" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/88/91834/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/miksery/tm-metabo/mikser-metabo-rwe-1020</t>
+  </si>
+  <si>
+    <t>63130</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/379404/</t>
+  </si>
+  <si>
+    <t>Дрель ударная "SBE 650" (Metabo) БЗП</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650</t>
+  </si>
+  <si>
+    <t>57550</t>
+  </si>
+  <si>
+    <t>Дрель ударная "SBE 650" (Metabo) ЗВП</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/263804/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650-1</t>
+  </si>
+  <si>
+    <t>57549</t>
+  </si>
+  <si>
+    <t>Лобзик "STEB 65 Quick" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/263805/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-65-quick</t>
+  </si>
+  <si>
+    <t>44087</t>
+  </si>
+  <si>
+    <t>Лобзик "STEB 70 Quick" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/248911/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-70-quick</t>
+  </si>
+  <si>
+    <t>83324</t>
+  </si>
+  <si>
+    <t>Лобзик акк. "STAB 18LTX100" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1057/106523/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki-akkumulyatornye/tm-metabo/akkumulatornyj-lobzik-metabo-stab-18-ltx-100-2</t>
+  </si>
+  <si>
+    <t>86113</t>
+  </si>
+  <si>
+    <t>Ножовка саб. акк. "SSE 18 LTX Compact" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/83/112017/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/sabelnye-pily-akkumulyatornye/tm-metabo/akkumulatornaa-sabelnaa-pila-metabo-sse-18-ltx-compact-2</t>
+  </si>
+  <si>
+    <t>78338</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная "SSE 1100" (Metabo) 1100Вт, 0-2600 об/мин, ход пилки 28 мм, 3,9 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/99/91838/</t>
+  </si>
+  <si>
+    <t>73825</t>
+  </si>
+  <si>
+    <t>Перфоратор "KHE 2444" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/3990314/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2444-2</t>
+  </si>
+  <si>
+    <t>82962</t>
+  </si>
+  <si>
+    <t>Перфоратор "KHE 2644" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/105538/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2644-2</t>
+  </si>
+  <si>
+    <t>85469</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "KS 305 M" (Metabo) 1600 Вт, диск 305*30 мм, ширина реза 200*140мм, глубина реза 102*60мм, лазер, подсветка, пылесборник, прижимное приспособление, 17 кг.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/111072/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-ks-305-m</t>
+  </si>
+  <si>
+    <t>44098</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "KS 216 M LASERCUT" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/248917/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-216-m-lasercut</t>
+  </si>
+  <si>
+    <t>70106</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "KGS 305M" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-305-m</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/403594/</t>
+  </si>
+  <si>
+    <t>44097</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "KGS 254 M" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/248916/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-254-m</t>
+  </si>
+  <si>
+    <t>72888</t>
+  </si>
+  <si>
+    <t>Пила ленточная "BAS 261" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/184/3799049/</t>
+  </si>
+  <si>
+    <t>78336</t>
+  </si>
+  <si>
+    <t>Пила дисковая акк. "KS 18 LTX" (Metabo) 18В, пропил 57 мм, диск 165*20 мм, 4600 об/мин, без АКК и ЗУ, коробка.</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-akkumulyatornye/tm-metabo/pila-diskovaa-akkumulatornaa-metabo-ks-18-ltx-57</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1059/91841/</t>
+  </si>
+  <si>
+    <t>46292</t>
+  </si>
+  <si>
+    <t>Пила дисковая "KS 55" (Metabo)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/251753/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-metabo/pila-diskovaya-metabo-ks-55</t>
+  </si>
+  <si>
+    <t>79950</t>
+  </si>
+  <si>
+    <t>Перфоратор акк. "KHA 18 LTX" (Metabo) 18В, 2,2Дж, 4000 об/мин, SDS-plus, 3 режима, без аккумуляторов и зарядки, в коробке.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1056/97909/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-akkumulyatornye/tm-metabo/perforator-akkumulatornyj-metabo-kha-18-ltx</t>
+  </si>
+  <si>
+    <t>70181</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/403593/</t>
+  </si>
+  <si>
+    <t>Перфоратор "KHE 2860 Quick" (Metabo) + патрон</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2860-quick</t>
+  </si>
+  <si>
+    <t>37263</t>
+  </si>
+  <si>
+    <t>Дрель "IE-1205 16/1300 ER" (Rebir)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/228274/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-rebir/drel-rebir-ie-1205-16-1300er</t>
+  </si>
+  <si>
+    <t>77081</t>
+  </si>
+  <si>
+    <t>Дрель "IE-1206-16/2000 ER" (Rebir) 2000 Вт, 0-330/0-500 об/мин, ЗВП, 6.3 кг</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/107788/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-rebir/drel-rebir-ie-1206-er</t>
+  </si>
+  <si>
+    <t>54142</t>
+  </si>
+  <si>
+    <t>Дрель "IE-1305 А-16/1300ER" (Rebir)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/346893/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-rebir/drel-rebir-ie-1305-16-1300r</t>
+  </si>
+  <si>
+    <t>61502</t>
+  </si>
+  <si>
+    <t>Пила дисковая "IE 5107G2" (Rebir)</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-rebir/pila-diskovaya-rebir-ie-5107-g2</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/346894/</t>
+  </si>
+  <si>
+    <t>11149</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/rubanki/rubanki-setevye/tm-rebir/rubanok-rebir-ie-5708c</t>
+  </si>
+  <si>
+    <t>Рубанок "IE-5708 C" (Rebir)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/255593/</t>
+  </si>
+  <si>
+    <t>28139</t>
+  </si>
+  <si>
+    <t>Шлифмашина прямая "TSM1-150" (Rebir)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/112/95995/</t>
+  </si>
+  <si>
+    <t>https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-pryamye/tm-rebir/shlifmashina-pryamaya-rebir-tsm-1-150</t>
   </si>
 </sst>
 </file>
@@ -1718,16 +3428,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:H284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D288" sqref="D288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="1025" width="11.5703125"/>
+    <col min="2" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2858,6 +4570,9 @@
       <c r="C80" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="D80" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
@@ -2911,6 +4626,9 @@
       <c r="C84" s="2" t="s">
         <v>291</v>
       </c>
+      <c r="D84" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
@@ -2922,6 +4640,9 @@
       <c r="C85" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="D85" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
@@ -3353,6 +5074,9 @@
       <c r="C116" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
@@ -3534,6 +5258,2176 @@
       </c>
       <c r="D129" s="2" t="s">
         <v>449</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B130" t="s">
+        <v>452</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B131" t="s">
+        <v>456</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B132" t="s">
+        <v>460</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B133" t="s">
+        <v>464</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B134" t="s">
+        <v>468</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B135" t="s">
+        <v>472</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B136" t="s">
+        <v>475</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="D136" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B137" t="s">
+        <v>478</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B138" t="s">
+        <v>482</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B139" t="s">
+        <v>485</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D139" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B140" t="s">
+        <v>488</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B141" t="s">
+        <v>492</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B142" t="s">
+        <v>496</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B143" t="s">
+        <v>500</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B144" t="s">
+        <v>504</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B145" t="s">
+        <v>508</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B146" t="s">
+        <v>512</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D146" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B147" t="s">
+        <v>515</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="D147" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B148" t="s">
+        <v>518</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B149" t="s">
+        <v>522</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B150" t="s">
+        <v>526</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B151" t="s">
+        <v>530</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D151" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B152" t="s">
+        <v>533</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B153" t="s">
+        <v>537</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="D153" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B154" t="s">
+        <v>540</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D154" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B155" t="s">
+        <v>543</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D155" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B156" t="s">
+        <v>546</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D156" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B157" t="s">
+        <v>549</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D157" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B158" t="s">
+        <v>552</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B159" t="s">
+        <v>556</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D159" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B160" t="s">
+        <v>559</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B161" t="s">
+        <v>563</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B162" t="s">
+        <v>567</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B163" t="s">
+        <v>571</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B164" t="s">
+        <v>575</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B165" t="s">
+        <v>579</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B166" t="s">
+        <v>583</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B167" t="s">
+        <v>587</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D167" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B168" t="s">
+        <v>590</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B169" t="s">
+        <v>594</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D169" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B170" t="s">
+        <v>597</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="D170" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B171" t="s">
+        <v>600</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B172" t="s">
+        <v>604</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B173" t="s">
+        <v>608</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B174" t="s">
+        <v>612</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D174" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B175" t="s">
+        <v>615</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B176" t="s">
+        <v>619</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B177" t="s">
+        <v>623</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D177" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B178" t="s">
+        <v>626</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B179" t="s">
+        <v>630</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="D179" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B180" t="s">
+        <v>633</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B181" t="s">
+        <v>637</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D181" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B182" t="s">
+        <v>640</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B183" t="s">
+        <v>644</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B184" t="s">
+        <v>648</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B185" t="s">
+        <v>652</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D185" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B186" t="s">
+        <v>655</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="D186" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B187" t="s">
+        <v>658</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B188" t="s">
+        <v>662</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B189" t="s">
+        <v>666</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B190" t="s">
+        <v>670</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="D190" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B191" t="s">
+        <v>673</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B192" t="s">
+        <v>677</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B193" t="s">
+        <v>681</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B194" t="s">
+        <v>685</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B195" t="s">
+        <v>689</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B196" t="s">
+        <v>693</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B197" t="s">
+        <v>697</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B198" t="s">
+        <v>701</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B199" t="s">
+        <v>705</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D199" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B200" t="s">
+        <v>708</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="B201" t="s">
+        <v>712</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B202" t="s">
+        <v>716</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="D202" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B203" t="s">
+        <v>719</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="D203" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B204" t="s">
+        <v>722</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="D204" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B205" t="s">
+        <v>725</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B206" t="s">
+        <v>729</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B207" t="s">
+        <v>733</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B208" t="s">
+        <v>737</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B209" t="s">
+        <v>741</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B210" t="s">
+        <v>745</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="D210" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B211" t="s">
+        <v>748</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B212" t="s">
+        <v>752</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B213" t="s">
+        <v>756</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B214" t="s">
+        <v>760</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B215" t="s">
+        <v>764</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B216" t="s">
+        <v>768</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D216" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B217" t="s">
+        <v>771</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B218" t="s">
+        <v>774</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B219" t="s">
+        <v>779</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D219" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B220" t="s">
+        <v>782</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="D220" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B221" t="s">
+        <v>785</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B222" t="s">
+        <v>789</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B223" t="s">
+        <v>793</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B224" t="s">
+        <v>797</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="D224" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B225" t="s">
+        <v>800</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B226" t="s">
+        <v>804</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="D226" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B227" t="s">
+        <v>807</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="D227" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B228" t="s">
+        <v>810</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B229" t="s">
+        <v>814</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B230" t="s">
+        <v>818</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B231" t="s">
+        <v>822</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B232" t="s">
+        <v>826</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B233" t="s">
+        <v>830</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="D233" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="B234" t="s">
+        <v>833</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B235" t="s">
+        <v>837</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="D235" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B236" t="s">
+        <v>840</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B237" t="s">
+        <v>844</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="D237" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B238" t="s">
+        <v>847</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="D238" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B239" t="s">
+        <v>850</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B240" t="s">
+        <v>854</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="D240" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B241" t="s">
+        <v>857</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B242" t="s">
+        <v>862</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="D242" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B243" t="s">
+        <v>864</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="D243" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B244" t="s">
+        <v>867</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B245" t="s">
+        <v>871</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B246" t="s">
+        <v>875</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D246" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B247" t="s">
+        <v>878</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B248" t="s">
+        <v>882</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B249" t="s">
+        <v>886</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="B250" t="s">
+        <v>890</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="D250" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B251" t="s">
+        <v>893</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B252" t="s">
+        <v>897</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B253" t="s">
+        <v>901</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="D253" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B254" t="s">
+        <v>904</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="D254" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B255" t="s">
+        <v>907</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="D255" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B256" t="s">
+        <v>910</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B257" t="s">
+        <v>914</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B258" t="s">
+        <v>918</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="D258" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B259" t="s">
+        <v>921</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="D259" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B260" t="s">
+        <v>924</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B261" t="s">
+        <v>929</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="B262" t="s">
+        <v>932</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B263" t="s">
+        <v>936</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B264" t="s">
+        <v>940</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B265" t="s">
+        <v>944</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B266" t="s">
+        <v>948</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="B267" t="s">
+        <v>952</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="D267" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B268" t="s">
+        <v>955</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="B269" t="s">
+        <v>959</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
+      <c r="A270" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B270" t="s">
+        <v>963</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
+      <c r="A271" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B271" t="s">
+        <v>967</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
+      <c r="A272" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B272" t="s">
+        <v>971</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4">
+      <c r="A273" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B273" t="s">
+        <v>975</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
+      <c r="A274" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B274" t="s">
+        <v>979</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="D274" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="B275" t="s">
+        <v>982</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="B276" t="s">
+        <v>986</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
+      <c r="A277" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B277" t="s">
+        <v>990</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
+      <c r="A278" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B278" t="s">
+        <v>995</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
+      <c r="A279" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B279" t="s">
+        <v>998</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -3733,9 +7627,272 @@
     <hyperlink ref="C129" r:id="rId193"/>
     <hyperlink ref="D129" r:id="rId194"/>
     <hyperlink ref="C79" r:id="rId195"/>
+    <hyperlink ref="D130" r:id="rId196"/>
+    <hyperlink ref="C130" r:id="rId197"/>
+    <hyperlink ref="C131" r:id="rId198"/>
+    <hyperlink ref="D131" r:id="rId199"/>
+    <hyperlink ref="C132" r:id="rId200"/>
+    <hyperlink ref="D132" r:id="rId201"/>
+    <hyperlink ref="C133" r:id="rId202"/>
+    <hyperlink ref="D133" r:id="rId203"/>
+    <hyperlink ref="C134" r:id="rId204"/>
+    <hyperlink ref="D134" r:id="rId205"/>
+    <hyperlink ref="C135" r:id="rId206"/>
+    <hyperlink ref="D135" r:id="rId207"/>
+    <hyperlink ref="C136" r:id="rId208"/>
+    <hyperlink ref="C137" r:id="rId209"/>
+    <hyperlink ref="D137" r:id="rId210"/>
+    <hyperlink ref="C138" r:id="rId211"/>
+    <hyperlink ref="C139" r:id="rId212"/>
+    <hyperlink ref="C140" r:id="rId213"/>
+    <hyperlink ref="D140" r:id="rId214"/>
+    <hyperlink ref="C141" r:id="rId215"/>
+    <hyperlink ref="D141" r:id="rId216"/>
+    <hyperlink ref="C142" r:id="rId217"/>
+    <hyperlink ref="D142" r:id="rId218"/>
+    <hyperlink ref="C143" r:id="rId219"/>
+    <hyperlink ref="D143" r:id="rId220"/>
+    <hyperlink ref="C144" r:id="rId221"/>
+    <hyperlink ref="D144" r:id="rId222"/>
+    <hyperlink ref="C145" r:id="rId223"/>
+    <hyperlink ref="D145" r:id="rId224"/>
+    <hyperlink ref="C146" r:id="rId225"/>
+    <hyperlink ref="C147" r:id="rId226"/>
+    <hyperlink ref="C148" r:id="rId227"/>
+    <hyperlink ref="D148" r:id="rId228"/>
+    <hyperlink ref="C149" r:id="rId229"/>
+    <hyperlink ref="D149" r:id="rId230"/>
+    <hyperlink ref="C150" r:id="rId231"/>
+    <hyperlink ref="D150" r:id="rId232"/>
+    <hyperlink ref="C151" r:id="rId233"/>
+    <hyperlink ref="C152" r:id="rId234"/>
+    <hyperlink ref="D152" r:id="rId235"/>
+    <hyperlink ref="C153" r:id="rId236"/>
+    <hyperlink ref="C154" r:id="rId237"/>
+    <hyperlink ref="C155" r:id="rId238"/>
+    <hyperlink ref="C156" r:id="rId239"/>
+    <hyperlink ref="C157" r:id="rId240"/>
+    <hyperlink ref="C158" r:id="rId241"/>
+    <hyperlink ref="D158" r:id="rId242"/>
+    <hyperlink ref="C159" r:id="rId243"/>
+    <hyperlink ref="C160" r:id="rId244"/>
+    <hyperlink ref="D160" r:id="rId245"/>
+    <hyperlink ref="C161" r:id="rId246"/>
+    <hyperlink ref="D161" r:id="rId247"/>
+    <hyperlink ref="C162" r:id="rId248"/>
+    <hyperlink ref="D162" r:id="rId249"/>
+    <hyperlink ref="C163" r:id="rId250"/>
+    <hyperlink ref="D163" r:id="rId251"/>
+    <hyperlink ref="C164" r:id="rId252"/>
+    <hyperlink ref="D164" r:id="rId253"/>
+    <hyperlink ref="C165" r:id="rId254"/>
+    <hyperlink ref="D165" r:id="rId255"/>
+    <hyperlink ref="C166" r:id="rId256"/>
+    <hyperlink ref="D166" r:id="rId257"/>
+    <hyperlink ref="C167" r:id="rId258"/>
+    <hyperlink ref="C168" r:id="rId259"/>
+    <hyperlink ref="D168" r:id="rId260"/>
+    <hyperlink ref="C169" r:id="rId261"/>
+    <hyperlink ref="C170" r:id="rId262"/>
+    <hyperlink ref="C171" r:id="rId263"/>
+    <hyperlink ref="D171" r:id="rId264"/>
+    <hyperlink ref="C172" r:id="rId265"/>
+    <hyperlink ref="D172" r:id="rId266"/>
+    <hyperlink ref="C173" r:id="rId267"/>
+    <hyperlink ref="D173" r:id="rId268"/>
+    <hyperlink ref="C174" r:id="rId269"/>
+    <hyperlink ref="C175" r:id="rId270"/>
+    <hyperlink ref="D175" r:id="rId271"/>
+    <hyperlink ref="C176" r:id="rId272"/>
+    <hyperlink ref="D176" r:id="rId273"/>
+    <hyperlink ref="C177" r:id="rId274"/>
+    <hyperlink ref="C178" r:id="rId275"/>
+    <hyperlink ref="D178" r:id="rId276"/>
+    <hyperlink ref="C179" r:id="rId277"/>
+    <hyperlink ref="C180" r:id="rId278"/>
+    <hyperlink ref="D180" r:id="rId279"/>
+    <hyperlink ref="C181" r:id="rId280"/>
+    <hyperlink ref="C182" r:id="rId281"/>
+    <hyperlink ref="D182" r:id="rId282"/>
+    <hyperlink ref="C183" r:id="rId283"/>
+    <hyperlink ref="D183" r:id="rId284"/>
+    <hyperlink ref="C184" r:id="rId285"/>
+    <hyperlink ref="D184" r:id="rId286"/>
+    <hyperlink ref="C185" r:id="rId287"/>
+    <hyperlink ref="C186" r:id="rId288"/>
+    <hyperlink ref="C187" r:id="rId289"/>
+    <hyperlink ref="D187" r:id="rId290"/>
+    <hyperlink ref="C188" r:id="rId291"/>
+    <hyperlink ref="D188" r:id="rId292"/>
+    <hyperlink ref="C189" r:id="rId293"/>
+    <hyperlink ref="D189" r:id="rId294"/>
+    <hyperlink ref="C190" r:id="rId295"/>
+    <hyperlink ref="C191" r:id="rId296"/>
+    <hyperlink ref="D191" r:id="rId297"/>
+    <hyperlink ref="C192" r:id="rId298"/>
+    <hyperlink ref="D192" r:id="rId299"/>
+    <hyperlink ref="C193" r:id="rId300"/>
+    <hyperlink ref="D193" r:id="rId301"/>
+    <hyperlink ref="C194" r:id="rId302"/>
+    <hyperlink ref="D194" r:id="rId303"/>
+    <hyperlink ref="C195" r:id="rId304"/>
+    <hyperlink ref="D195" r:id="rId305"/>
+    <hyperlink ref="C196" r:id="rId306"/>
+    <hyperlink ref="D196" r:id="rId307"/>
+    <hyperlink ref="C197" r:id="rId308"/>
+    <hyperlink ref="D197" r:id="rId309"/>
+    <hyperlink ref="C198" r:id="rId310"/>
+    <hyperlink ref="D198" r:id="rId311"/>
+    <hyperlink ref="C199" r:id="rId312"/>
+    <hyperlink ref="C200" r:id="rId313"/>
+    <hyperlink ref="D200" r:id="rId314"/>
+    <hyperlink ref="C201" r:id="rId315"/>
+    <hyperlink ref="D201" r:id="rId316"/>
+    <hyperlink ref="C202" r:id="rId317"/>
+    <hyperlink ref="C203" r:id="rId318"/>
+    <hyperlink ref="C204" r:id="rId319"/>
+    <hyperlink ref="C205" r:id="rId320"/>
+    <hyperlink ref="D205" r:id="rId321"/>
+    <hyperlink ref="C206" r:id="rId322"/>
+    <hyperlink ref="D206" r:id="rId323"/>
+    <hyperlink ref="C207" r:id="rId324"/>
+    <hyperlink ref="D207" r:id="rId325"/>
+    <hyperlink ref="C208" r:id="rId326"/>
+    <hyperlink ref="D208" r:id="rId327"/>
+    <hyperlink ref="C209" r:id="rId328"/>
+    <hyperlink ref="D209" r:id="rId329"/>
+    <hyperlink ref="C210" r:id="rId330"/>
+    <hyperlink ref="C211" r:id="rId331"/>
+    <hyperlink ref="D211" r:id="rId332"/>
+    <hyperlink ref="C212" r:id="rId333"/>
+    <hyperlink ref="D212" r:id="rId334"/>
+    <hyperlink ref="C213" r:id="rId335"/>
+    <hyperlink ref="D213" r:id="rId336"/>
+    <hyperlink ref="C214" r:id="rId337"/>
+    <hyperlink ref="D214" r:id="rId338"/>
+    <hyperlink ref="C215" r:id="rId339"/>
+    <hyperlink ref="D215" r:id="rId340"/>
+    <hyperlink ref="C216" r:id="rId341"/>
+    <hyperlink ref="C217" r:id="rId342"/>
+    <hyperlink ref="C218" r:id="rId343"/>
+    <hyperlink ref="D217" r:id="rId344"/>
+    <hyperlink ref="D218" r:id="rId345"/>
+    <hyperlink ref="C219" r:id="rId346"/>
+    <hyperlink ref="C220" r:id="rId347"/>
+    <hyperlink ref="C221" r:id="rId348"/>
+    <hyperlink ref="D221" r:id="rId349"/>
+    <hyperlink ref="C222" r:id="rId350"/>
+    <hyperlink ref="D222" r:id="rId351"/>
+    <hyperlink ref="C223" r:id="rId352"/>
+    <hyperlink ref="D223" r:id="rId353"/>
+    <hyperlink ref="C224" r:id="rId354"/>
+    <hyperlink ref="C225" r:id="rId355"/>
+    <hyperlink ref="D225" r:id="rId356"/>
+    <hyperlink ref="C226" r:id="rId357"/>
+    <hyperlink ref="C227" r:id="rId358"/>
+    <hyperlink ref="C228" r:id="rId359"/>
+    <hyperlink ref="D228" r:id="rId360"/>
+    <hyperlink ref="C229" r:id="rId361"/>
+    <hyperlink ref="D229" r:id="rId362"/>
+    <hyperlink ref="D230" r:id="rId363"/>
+    <hyperlink ref="C230" r:id="rId364"/>
+    <hyperlink ref="C231" r:id="rId365"/>
+    <hyperlink ref="D231" r:id="rId366"/>
+    <hyperlink ref="C232" r:id="rId367"/>
+    <hyperlink ref="D232" r:id="rId368"/>
+    <hyperlink ref="C233" r:id="rId369"/>
+    <hyperlink ref="C234" r:id="rId370"/>
+    <hyperlink ref="D234" r:id="rId371"/>
+    <hyperlink ref="C235" r:id="rId372"/>
+    <hyperlink ref="C236" r:id="rId373"/>
+    <hyperlink ref="D236" r:id="rId374"/>
+    <hyperlink ref="C237" r:id="rId375"/>
+    <hyperlink ref="C238" r:id="rId376"/>
+    <hyperlink ref="C239" r:id="rId377"/>
+    <hyperlink ref="D239" r:id="rId378"/>
+    <hyperlink ref="C240" r:id="rId379"/>
+    <hyperlink ref="C241" r:id="rId380"/>
+    <hyperlink ref="D241" r:id="rId381"/>
+    <hyperlink ref="B242" r:id="rId382" display="https://stroybatinfo.ru/catalog/113/403595/"/>
+    <hyperlink ref="C242" r:id="rId383"/>
+    <hyperlink ref="C243" r:id="rId384"/>
+    <hyperlink ref="C244" r:id="rId385"/>
+    <hyperlink ref="D244" r:id="rId386"/>
+    <hyperlink ref="C245" r:id="rId387"/>
+    <hyperlink ref="D245" r:id="rId388"/>
+    <hyperlink ref="C246" r:id="rId389"/>
+    <hyperlink ref="C247" r:id="rId390"/>
+    <hyperlink ref="D247" r:id="rId391"/>
+    <hyperlink ref="C248" r:id="rId392"/>
+    <hyperlink ref="D248" r:id="rId393"/>
+    <hyperlink ref="C249" r:id="rId394"/>
+    <hyperlink ref="D249" r:id="rId395"/>
+    <hyperlink ref="C250" r:id="rId396"/>
+    <hyperlink ref="C251" r:id="rId397"/>
+    <hyperlink ref="D251" r:id="rId398"/>
+    <hyperlink ref="C252" r:id="rId399"/>
+    <hyperlink ref="D252" r:id="rId400"/>
+    <hyperlink ref="C253" r:id="rId401"/>
+    <hyperlink ref="C254" r:id="rId402"/>
+    <hyperlink ref="C255" r:id="rId403"/>
+    <hyperlink ref="C256" r:id="rId404"/>
+    <hyperlink ref="D256" r:id="rId405"/>
+    <hyperlink ref="C257" r:id="rId406"/>
+    <hyperlink ref="D257" r:id="rId407"/>
+    <hyperlink ref="C258" r:id="rId408"/>
+    <hyperlink ref="C259" r:id="rId409"/>
+    <hyperlink ref="C260" r:id="rId410"/>
+    <hyperlink ref="D260" r:id="rId411"/>
+    <hyperlink ref="C261" r:id="rId412"/>
+    <hyperlink ref="D261" r:id="rId413"/>
+    <hyperlink ref="C262" r:id="rId414"/>
+    <hyperlink ref="D262" r:id="rId415"/>
+    <hyperlink ref="C263" r:id="rId416"/>
+    <hyperlink ref="D263" r:id="rId417"/>
+    <hyperlink ref="C264" r:id="rId418"/>
+    <hyperlink ref="D264" r:id="rId419"/>
+    <hyperlink ref="C265" r:id="rId420"/>
+    <hyperlink ref="D265" r:id="rId421"/>
+    <hyperlink ref="C266" r:id="rId422"/>
+    <hyperlink ref="D266" r:id="rId423"/>
+    <hyperlink ref="C267" r:id="rId424"/>
+    <hyperlink ref="C268" r:id="rId425"/>
+    <hyperlink ref="D268" r:id="rId426"/>
+    <hyperlink ref="C269" r:id="rId427"/>
+    <hyperlink ref="D269" r:id="rId428"/>
+    <hyperlink ref="C270" r:id="rId429"/>
+    <hyperlink ref="D270" r:id="rId430"/>
+    <hyperlink ref="C271" r:id="rId431"/>
+    <hyperlink ref="D271" r:id="rId432"/>
+    <hyperlink ref="D272" r:id="rId433"/>
+    <hyperlink ref="C272" r:id="rId434"/>
+    <hyperlink ref="C273" r:id="rId435"/>
+    <hyperlink ref="D273" r:id="rId436"/>
+    <hyperlink ref="C274" r:id="rId437"/>
+    <hyperlink ref="D275" r:id="rId438"/>
+    <hyperlink ref="C275" r:id="rId439"/>
+    <hyperlink ref="C276" r:id="rId440"/>
+    <hyperlink ref="D276" r:id="rId441"/>
+    <hyperlink ref="C277" r:id="rId442"/>
+    <hyperlink ref="D277" r:id="rId443"/>
+    <hyperlink ref="B278" r:id="rId444" display="https://stroybatinfo.ru/catalog/91/403593/"/>
+    <hyperlink ref="C278" r:id="rId445"/>
+    <hyperlink ref="D278" r:id="rId446"/>
+    <hyperlink ref="C279" r:id="rId447"/>
+    <hyperlink ref="D279" r:id="rId448"/>
+    <hyperlink ref="C280" r:id="rId449"/>
+    <hyperlink ref="D280" r:id="rId450"/>
+    <hyperlink ref="C281" r:id="rId451"/>
+    <hyperlink ref="D281" r:id="rId452"/>
+    <hyperlink ref="D282" r:id="rId453"/>
+    <hyperlink ref="C282" r:id="rId454"/>
+    <hyperlink ref="D283" r:id="rId455"/>
+    <hyperlink ref="C283" r:id="rId456"/>
+    <hyperlink ref="C284" r:id="rId457"/>
+    <hyperlink ref="D284" r:id="rId458"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId196"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId459"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>